<commit_message>
Fixed Rate Done Initially
</commit_message>
<xml_diff>
--- a/DOC/Profit.xlsx
+++ b/DOC/Profit.xlsx
@@ -174,7 +174,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -229,7 +229,7 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:L22"/>
+  <dimension ref="C1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,18 +528,19 @@
     <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E1" s="1"/>
       <c r="J1"/>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
       <c r="J2"/>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -557,14 +558,14 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -582,7 +583,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
       <c r="I6" s="1"/>
@@ -592,7 +593,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -614,14 +615,14 @@
         <v>365</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
       <c r="G8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>2</v>
       </c>
@@ -631,7 +632,7 @@
       <c r="J9"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>3</v>
       </c>
@@ -641,14 +642,14 @@
       <c r="J10"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
       <c r="G11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>5</v>
       </c>
@@ -670,7 +671,7 @@
         <v>15068.493150684932</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>360</v>
       </c>
@@ -679,46 +680,39 @@
         <v>5500000</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="3">
-        <f>DATE(2020,2,1)</f>
-        <v>43862</v>
-      </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+        <f>DATE(2020,11,1)</f>
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="3">
-        <f>DATE(2020,12,30)</f>
-        <v>44195</v>
-      </c>
+        <f>DATE(2020,11,25)</f>
+        <v>44160</v>
+      </c>
+      <c r="P16" s="4"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17">
         <f>E16-E15</f>
-        <v>333</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="4">
         <f>E17*E12</f>
-        <v>5087500</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19">
-        <v>5087500</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="4">
-        <f>E19-E18</f>
-        <v>0</v>
-      </c>
+        <v>366666.66666666663</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>